<commit_message>
re-generate country profiles adding item id
</commit_message>
<xml_diff>
--- a/unsd/country-profiles/ProjectCountryProfilesPython/CountryProfileBuilder.xlsx
+++ b/unsd/country-profiles/ProjectCountryProfilesPython/CountryProfileBuilder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\unsd\country-profiles\ProjectCountryProfilesPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68BFC46-C238-40A8-AA30-7ECCCFD4B098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F31823-35D6-43DE-B18C-597D795D8591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" xr2:uid="{608E191F-5FEB-4D0E-811F-33218E7FD720}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CountryProfileBuilder" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AG$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AH$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="346">
   <si>
     <t>No.</t>
   </si>
@@ -930,6 +930,147 @@
   </si>
   <si>
     <t>Up</t>
+  </si>
+  <si>
+    <t>ed6ee35ad584405b8f3ef2abc22f6948</t>
+  </si>
+  <si>
+    <t>HubItemId</t>
+  </si>
+  <si>
+    <t>deb1f4a7e2e14d78a113c53cba2838de</t>
+  </si>
+  <si>
+    <t>f4cb37d065aa4b6981d93e8266f63fd0</t>
+  </si>
+  <si>
+    <t>8c0866ad73ae486ba647f5490fed5529</t>
+  </si>
+  <si>
+    <t>30ea76b4f4094d4aa7645a213ccaa4b9</t>
+  </si>
+  <si>
+    <t>65925035bb984f66aa03480f6754c4fe</t>
+  </si>
+  <si>
+    <t>a012070afbd3486d9c0596352b9698d6</t>
+  </si>
+  <si>
+    <t>216c7516b9444f289e8f7910c8726e9f</t>
+  </si>
+  <si>
+    <t>954b5087e440421ba26a3213c99d9a9f</t>
+  </si>
+  <si>
+    <t>1a967f6f5fe64fc5b27f49a5c20e4fe4</t>
+  </si>
+  <si>
+    <t>0c846dfa5bab411c9a1a21ae40dd0232</t>
+  </si>
+  <si>
+    <t>dc8f11cd784344f18d0478072691b943</t>
+  </si>
+  <si>
+    <t>512b7b1d05a14b90853ea5ca1d003b1b</t>
+  </si>
+  <si>
+    <t>c24e8fbbada54780b6c36fd899f864b2</t>
+  </si>
+  <si>
+    <t>7f75a26e77c7487e993799b22ad7ba88</t>
+  </si>
+  <si>
+    <t>8f2dd8895e1242db8ef4ca25415d609d</t>
+  </si>
+  <si>
+    <t>3459681b792a4979a9d9731c75f7f80d</t>
+  </si>
+  <si>
+    <t>32abbaca0c3a47c0aae18f50bd7e8f56</t>
+  </si>
+  <si>
+    <t>337524c727bd498c8726f9f6bc6512e1</t>
+  </si>
+  <si>
+    <t>2186448878244705a5295710c140b8c3</t>
+  </si>
+  <si>
+    <t>8f37f35525db476a9da37c7d83beffa9</t>
+  </si>
+  <si>
+    <t>28a9a3072fd940aa9fb0f983d25ef65f</t>
+  </si>
+  <si>
+    <t>9fd0677f368c48dca6f5e11f64badafd</t>
+  </si>
+  <si>
+    <t>b087399f0b874ab9948714edcd49cbdd</t>
+  </si>
+  <si>
+    <t>81cf3e70351c4895828a2486efa2142c</t>
+  </si>
+  <si>
+    <t>3cb997d2497148e68dca6787fcb84ca5</t>
+  </si>
+  <si>
+    <t>72c32323563d4a0b9432c9edcb85267a</t>
+  </si>
+  <si>
+    <t>b5ff535a5fa841659c576685489dfac7</t>
+  </si>
+  <si>
+    <t>a4e6d6a6cc804c3598cc9b96cd96ce67</t>
+  </si>
+  <si>
+    <t>8943ce6f81b44120b6124fedb3b094d8</t>
+  </si>
+  <si>
+    <t>635cd0cae73e4b2dae2661407be6eeec</t>
+  </si>
+  <si>
+    <t>5b43bb59961a46daa3b8af9384f60103</t>
+  </si>
+  <si>
+    <t>f158f819bd284fd5b35e456a152a069c</t>
+  </si>
+  <si>
+    <t>995242b2ec9f4a21975ef7d47b5657bb</t>
+  </si>
+  <si>
+    <t>9c33807e2ddf4e348737fab085de0ac1</t>
+  </si>
+  <si>
+    <t>d675ccc2f7054d82b371e64fb2cbface</t>
+  </si>
+  <si>
+    <t>2a0cad7f76284e8c978bfcb0fa15cd76</t>
+  </si>
+  <si>
+    <t>e23061ce674142b5b33c46ea5e031658</t>
+  </si>
+  <si>
+    <t>5c12290ecd1c4a49bc3734721d941d10</t>
+  </si>
+  <si>
+    <t>c2c0216c53744dd7b5278e398328bc99</t>
+  </si>
+  <si>
+    <t>b65e89e905a744e5992889ddc27f8fc7</t>
+  </si>
+  <si>
+    <t>f16a0c0c54504a84bd7296f42375d73e</t>
+  </si>
+  <si>
+    <t>f59cf3f8a0ec41a2b601a28682e6f2c8</t>
+  </si>
+  <si>
+    <t>bc201a5c69e94e23b45bad86c828f1be</t>
+  </si>
+  <si>
+    <t>4da2587ef9094c7bb1e2980644211cf2</t>
+  </si>
+  <si>
+    <t>68e9ec78abe543889762bbdd36cd3d31</t>
   </si>
 </sst>
 </file>
@@ -945,12 +1086,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -965,13 +1112,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,38 +1437,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BF65AC-2E6C-4B3F-8D19-434C6AC10D50}">
-  <dimension ref="A1:Z57"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="56.85546875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="56.85546875" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1329,76 +1480,79 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1408,47 +1562,50 @@
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
+      <c r="D2" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="1">
-        <v>1</v>
-      </c>
       <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>26</v>
+      <c r="S2" s="1">
+        <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1458,53 +1615,56 @@
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
+      <c r="D3" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
       <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
         <v>2</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1514,47 +1674,50 @@
       <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
+      <c r="D4" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
       <c r="R4" s="1">
         <v>1</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1564,53 +1727,56 @@
       <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
+      <c r="D5" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="1">
-        <v>1</v>
-      </c>
       <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
         <v>2</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1620,26 +1786,29 @@
       <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1649,47 +1818,50 @@
       <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
+      <c r="D7" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <v>0</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>7</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="U7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="AA7" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1699,53 +1871,56 @@
       <c r="C8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
+      <c r="D8" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="1">
-        <v>1</v>
-      </c>
       <c r="R8" s="1">
         <v>1</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>26</v>
+      <c r="S8" s="1">
+        <v>1</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="U8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1755,53 +1930,56 @@
       <c r="C9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
+      <c r="D9" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <v>0</v>
       </c>
-      <c r="R9" s="1">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1" t="s">
+      <c r="S9" s="1">
+        <v>1</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="AA9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1811,53 +1989,56 @@
       <c r="C10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
+      <c r="D10" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="1">
-        <v>1</v>
-      </c>
       <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
         <v>13</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="Y10" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1867,23 +2048,26 @@
       <c r="C11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="1">
+      <c r="D11" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1893,47 +2077,50 @@
       <c r="C12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
+      <c r="D12" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <v>0</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>14</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="X12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Z12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z12" s="2" t="s">
+      <c r="AA12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1943,23 +2130,26 @@
       <c r="C13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="1">
+      <c r="D13" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>56</v>
       </c>
@@ -1969,50 +2159,53 @@
       <c r="C14" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
+      <c r="D14" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <v>0</v>
       </c>
-      <c r="R14" s="1">
-        <v>1</v>
-      </c>
-      <c r="S14" s="1" t="s">
+      <c r="S14" s="1">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="AA14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2022,44 +2215,47 @@
       <c r="C15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="1">
-        <v>1</v>
+      <c r="D15" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
         <v>4</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>0</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>4</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="V15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="V15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="Y15" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2069,44 +2265,47 @@
       <c r="C16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="1">
-        <v>1</v>
+      <c r="D16" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>0</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <v>4</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="V16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="V16" s="2" t="s">
+      <c r="W16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="X16" s="2" t="s">
+      <c r="Y16" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2116,44 +2315,47 @@
       <c r="C17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="1">
+      <c r="D17" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F17" s="1">
         <v>4</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <v>0</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="V17" s="2" t="s">
+      <c r="W17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Y17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="AA17" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>57</v>
       </c>
@@ -2163,47 +2365,50 @@
       <c r="C18" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D18" s="1">
-        <v>1</v>
+      <c r="D18" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
         <v>4</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <v>0</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <v>2</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="V18" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="AA18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -2213,26 +2418,29 @@
       <c r="C19" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="1">
+      <c r="D19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F19" s="1">
         <v>5</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="R19" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -2242,47 +2450,50 @@
       <c r="C20" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="1">
-        <v>1</v>
+      <c r="D20" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
         <v>5</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <v>0</v>
       </c>
-      <c r="R20" s="1">
-        <v>1</v>
-      </c>
-      <c r="S20" s="1" t="s">
+      <c r="S20" s="1">
+        <v>1</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="V20" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="X20" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="Y20" s="2" t="s">
+      <c r="Z20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z20" s="2" t="s">
+      <c r="AA20" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2292,50 +2503,53 @@
       <c r="C21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="1">
-        <v>1</v>
+      <c r="D21" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
         <v>5</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <v>0</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S21" s="1">
         <v>2</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="V21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="X21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z21" s="2" t="s">
+      <c r="AA21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2345,26 +2559,29 @@
       <c r="C22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="1">
+      <c r="D22" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F22" s="1">
         <v>6</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -2374,44 +2591,47 @@
       <c r="C23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="1">
+      <c r="D23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F23" s="1">
         <v>6</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q23" s="1">
-        <v>1</v>
-      </c>
       <c r="R23" s="1">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1">
         <v>2</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="V23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Z23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z23" s="2" t="s">
+      <c r="AA23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2421,26 +2641,29 @@
       <c r="C24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="1">
+      <c r="D24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F24" s="1">
         <v>6</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -2450,32 +2673,35 @@
       <c r="C25" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="1">
+      <c r="D25" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" s="1">
         <v>6</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="R25" s="1">
         <v>0</v>
       </c>
-      <c r="Y25" s="2" t="s">
+      <c r="Z25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z25" s="2" t="s">
+      <c r="AA25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -2485,47 +2711,50 @@
       <c r="C26" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="1">
-        <v>1</v>
+      <c r="D26" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
         <v>6</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="R26" s="1">
         <v>0</v>
       </c>
-      <c r="R26" s="1">
+      <c r="S26" s="1">
         <v>2</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="V26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="W26" s="2" t="s">
+      <c r="X26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Y26" s="2" t="s">
+      <c r="Z26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z26" s="2" t="s">
+      <c r="AA26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -2535,26 +2764,29 @@
       <c r="C27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="1">
+      <c r="D27" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F27" s="1">
         <v>6</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -2564,47 +2796,50 @@
       <c r="C28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="1">
-        <v>1</v>
+      <c r="D28" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
         <v>6</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="R28" s="1">
         <v>0</v>
       </c>
-      <c r="R28" s="1">
+      <c r="S28" s="1">
         <v>2</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="V28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W28" s="2" t="s">
+      <c r="X28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="Y28" s="2" t="s">
+      <c r="Z28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z28" s="2" t="s">
+      <c r="AA28" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -2614,38 +2849,41 @@
       <c r="C29" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D29" s="1">
-        <v>1</v>
+      <c r="D29" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="R29" s="1">
         <v>0</v>
       </c>
-      <c r="R29" s="1">
+      <c r="S29" s="1">
         <v>8</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="V29" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="W29" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -2655,47 +2893,50 @@
       <c r="C30" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="1">
-        <v>1</v>
+      <c r="D30" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
         <v>7</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="R30" s="1">
         <v>0</v>
       </c>
-      <c r="R30" s="1">
-        <v>1</v>
-      </c>
-      <c r="S30" s="1" t="s">
+      <c r="S30" s="1">
+        <v>1</v>
+      </c>
+      <c r="T30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="V30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="W30" s="2" t="s">
+      <c r="X30" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="Y30" s="2" t="s">
+      <c r="Z30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z30" s="2" t="s">
+      <c r="AA30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2705,44 +2946,47 @@
       <c r="C31" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="1">
-        <v>1</v>
+      <c r="D31" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
         <v>8</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="R31" s="1">
         <v>0</v>
       </c>
-      <c r="R31" s="1">
-        <v>1</v>
-      </c>
-      <c r="S31" s="1" t="s">
+      <c r="S31" s="1">
+        <v>1</v>
+      </c>
+      <c r="T31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="V31" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="W31" s="2" t="s">
+      <c r="X31" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y31" s="2" t="s">
+      <c r="Z31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z31" s="2" t="s">
+      <c r="AA31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2752,29 +2996,32 @@
       <c r="C32" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E32" s="1">
+      <c r="D32" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F32" s="1">
         <v>8</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="R32" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2784,29 +3031,32 @@
       <c r="C33" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E33" s="1">
+      <c r="D33" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F33" s="1">
         <v>8</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="R33" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2816,29 +3066,32 @@
       <c r="C34" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E34" s="1">
+      <c r="D34" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F34" s="1">
         <v>8</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="R34" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2848,50 +3101,53 @@
       <c r="C35" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D35" s="1">
-        <v>1</v>
+      <c r="D35" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
         <v>8</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="R35" s="1">
         <v>0</v>
       </c>
-      <c r="R35" s="1">
-        <v>1</v>
-      </c>
-      <c r="S35" s="1" t="s">
+      <c r="S35" s="1">
+        <v>1</v>
+      </c>
+      <c r="T35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U35" s="2" t="s">
+      <c r="V35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="W35" s="2" t="s">
+      <c r="X35" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="Y35" s="2" t="s">
+      <c r="Z35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z35" s="2" t="s">
+      <c r="AA35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2901,29 +3157,32 @@
       <c r="C36" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E36" s="1">
+      <c r="D36" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F36" s="1">
         <v>8</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="R36" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2933,44 +3192,47 @@
       <c r="C37" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D37" s="1">
-        <v>1</v>
+      <c r="D37" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
         <v>9</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="R37" s="1">
         <v>0</v>
       </c>
-      <c r="R37" s="1">
-        <v>1</v>
-      </c>
-      <c r="S37" s="1" t="s">
+      <c r="S37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="V37" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="W37" s="2" t="s">
+      <c r="X37" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Y37" s="2" t="s">
+      <c r="Z37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z37" s="2" t="s">
+      <c r="AA37" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2980,47 +3242,50 @@
       <c r="C38" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D38" s="1">
-        <v>1</v>
+      <c r="D38" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
         <v>9</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="R38" s="1">
         <v>0</v>
       </c>
-      <c r="R38" s="1">
+      <c r="S38" s="1">
         <v>9</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="U38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U38" s="2" t="s">
+      <c r="V38" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="W38" s="2" t="s">
+      <c r="X38" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="Y38" s="2" t="s">
+      <c r="Z38" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Z38" s="2" t="s">
+      <c r="AA38" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3030,47 +3295,50 @@
       <c r="C39" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D39" s="1">
-        <v>1</v>
+      <c r="D39" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
         <v>9</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="R39" s="1">
         <v>0</v>
       </c>
-      <c r="R39" s="1">
+      <c r="S39" s="1">
         <v>2</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U39" s="2" t="s">
+      <c r="V39" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="W39" s="2" t="s">
+      <c r="X39" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="Y39" s="2" t="s">
+      <c r="Z39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z39" s="2" t="s">
+      <c r="AA39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -3080,44 +3348,47 @@
       <c r="C40" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D40" s="1">
-        <v>1</v>
+      <c r="D40" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
         <v>10</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="R40" s="1">
         <v>0</v>
       </c>
-      <c r="R40" s="1">
+      <c r="S40" s="1">
         <v>2</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U40" s="2" t="s">
+      <c r="V40" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W40" s="2" t="s">
+      <c r="X40" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="Y40" s="2" t="s">
+      <c r="Z40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Z40" s="2" t="s">
+      <c r="AA40" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -3127,47 +3398,50 @@
       <c r="C41" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D41" s="1">
-        <v>1</v>
+      <c r="D41" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
         <v>11</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="R41" s="1">
         <v>0</v>
       </c>
-      <c r="R41" s="1">
+      <c r="S41" s="1">
         <v>10</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="U41" s="2" t="s">
+      <c r="V41" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="W41" s="2" t="s">
+      <c r="X41" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="Y41" s="2" t="s">
+      <c r="Z41" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="Z41" s="2" t="s">
+      <c r="AA41" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -3177,26 +3451,29 @@
       <c r="C42" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E42" s="1">
+      <c r="D42" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F42" s="1">
         <v>11</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="R42" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -3206,44 +3483,47 @@
       <c r="C43" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D43" s="1">
-        <v>1</v>
+      <c r="D43" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
         <v>11</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="R43" s="1">
         <v>0</v>
       </c>
-      <c r="R43" s="1">
-        <v>1</v>
-      </c>
-      <c r="S43" s="1" t="s">
+      <c r="S43" s="1">
+        <v>1</v>
+      </c>
+      <c r="T43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U43" s="2" t="s">
+      <c r="V43" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W43" s="2" t="s">
+      <c r="X43" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="Y43" s="2" t="s">
+      <c r="Z43" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="Z43" s="2" t="s">
+      <c r="AA43" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>28</v>
       </c>
@@ -3253,47 +3533,50 @@
       <c r="C44" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D44" s="1">
-        <v>1</v>
+      <c r="D44" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
         <v>12</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="Q44" s="1">
-        <v>1</v>
-      </c>
       <c r="R44" s="1">
         <v>1</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="S44" s="1">
+        <v>1</v>
+      </c>
+      <c r="T44" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="U44" s="2" t="s">
+      <c r="V44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="W44" s="2" t="s">
+      <c r="X44" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="Y44" s="2" t="s">
+      <c r="Z44" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z44" s="2" t="s">
+      <c r="AA44" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>29</v>
       </c>
@@ -3303,38 +3586,41 @@
       <c r="C45" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E45" s="1">
+      <c r="D45" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F45" s="1">
         <v>12</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="Q45" s="1">
-        <v>1</v>
-      </c>
       <c r="R45" s="1">
+        <v>1</v>
+      </c>
+      <c r="S45" s="1">
         <v>7</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="V45" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="W45" s="2" t="s">
+      <c r="X45" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>55</v>
       </c>
@@ -3344,38 +3630,41 @@
       <c r="C46" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D46" s="1">
-        <v>1</v>
+      <c r="D46" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
         <v>13</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="R46" s="1">
         <v>0</v>
       </c>
-      <c r="R46" s="1">
+      <c r="S46" s="1">
         <v>12</v>
       </c>
-      <c r="W46" s="2" t="s">
+      <c r="X46" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="Y46" s="2" t="s">
+      <c r="Z46" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="Z46" s="2" t="s">
+      <c r="AA46" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44</v>
       </c>
@@ -3385,38 +3674,41 @@
       <c r="C47" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D47" s="1">
-        <v>1</v>
+      <c r="D47" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
         <v>14</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="Q47" s="1">
-        <v>1</v>
-      </c>
       <c r="R47" s="1">
+        <v>1</v>
+      </c>
+      <c r="S47" s="1">
         <v>8</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="V47" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="X47" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45</v>
       </c>
@@ -3426,44 +3718,47 @@
       <c r="C48" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D48" s="1">
-        <v>1</v>
+      <c r="D48" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
         <v>15</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="Q48" s="1">
-        <v>1</v>
-      </c>
       <c r="R48" s="1">
         <v>1</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="S48" s="1">
+        <v>1</v>
+      </c>
+      <c r="T48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="V48" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="W48" s="2" t="s">
+      <c r="X48" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="Y48" s="2" t="s">
+      <c r="Z48" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="Z48" s="2" t="s">
+      <c r="AA48" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -3473,41 +3768,44 @@
       <c r="C49" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D49" s="1">
-        <v>1</v>
+      <c r="D49" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
         <v>15</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q49" s="1">
-        <v>1</v>
-      </c>
       <c r="R49" s="1">
+        <v>1</v>
+      </c>
+      <c r="S49" s="1">
         <v>7</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U49" s="2" t="s">
+      <c r="V49" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="W49" s="2" t="s">
+      <c r="X49" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3517,41 +3815,44 @@
       <c r="C50" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D50" s="1">
-        <v>1</v>
+      <c r="D50" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
         <v>15</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q50" s="1">
-        <v>1</v>
-      </c>
       <c r="R50" s="1">
+        <v>1</v>
+      </c>
+      <c r="S50" s="1">
         <v>7</v>
       </c>
-      <c r="S50" s="1" t="s">
+      <c r="T50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U50" s="2" t="s">
+      <c r="V50" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="W50" s="2" t="s">
+      <c r="X50" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3561,47 +3862,48 @@
       <c r="C51" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
+      <c r="D51" s="3"/>
       <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
         <v>16</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q51" s="1">
+      <c r="R51" s="1">
         <v>0</v>
       </c>
-      <c r="R51" s="1">
+      <c r="S51" s="1">
         <v>3</v>
       </c>
-      <c r="S51" s="1" t="s">
+      <c r="T51" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U51" s="2" t="s">
+      <c r="V51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="V51" s="2" t="s">
+      <c r="W51" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="W51" s="2" t="s">
+      <c r="X51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="X51" s="2" t="s">
+      <c r="Y51" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3611,38 +3913,41 @@
       <c r="C52" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D52" s="1">
-        <v>1</v>
+      <c r="D52" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
         <v>16</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="R52" s="1">
         <v>0</v>
       </c>
-      <c r="R52" s="1">
+      <c r="S52" s="1">
         <v>11</v>
       </c>
-      <c r="S52" s="1" t="s">
+      <c r="T52" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="U52" s="2" t="s">
+      <c r="V52" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="W52" s="2" t="s">
+      <c r="X52" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3652,47 +3957,50 @@
       <c r="C53" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D53" s="1">
-        <v>1</v>
+      <c r="D53" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
         <v>17</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="Q53" s="1">
-        <v>1</v>
-      </c>
       <c r="R53" s="1">
         <v>1</v>
       </c>
-      <c r="S53" s="1" t="s">
-        <v>26</v>
+      <c r="S53" s="1">
+        <v>1</v>
       </c>
       <c r="T53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U53" s="2" t="s">
+      <c r="U53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V53" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="W53" s="2" t="s">
+      <c r="X53" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="Y53" s="2" t="s">
+      <c r="Z53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z53" s="2" t="s">
+      <c r="AA53" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3702,50 +4010,53 @@
       <c r="C54" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D54" s="1">
-        <v>1</v>
+      <c r="D54" s="1" t="s">
+        <v>342</v>
       </c>
       <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
         <v>17</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="P54" s="1" t="s">
+      <c r="Q54" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="Q54" s="1">
+      <c r="R54" s="1">
         <v>0</v>
       </c>
-      <c r="R54" s="1">
+      <c r="S54" s="1">
         <v>15</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="T54" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U54" s="2" t="s">
+      <c r="V54" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="W54" s="2" t="s">
+      <c r="X54" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="Y54" s="2" t="s">
+      <c r="Z54" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z54" s="2" t="s">
+      <c r="AA54" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3755,38 +4066,41 @@
       <c r="C55" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D55" s="1">
-        <v>1</v>
+      <c r="D55" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
         <v>17</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="Q55" s="1">
+      <c r="R55" s="1">
         <v>0</v>
       </c>
-      <c r="R55" s="1">
+      <c r="S55" s="1">
         <v>12</v>
       </c>
-      <c r="W55" s="2" t="s">
+      <c r="X55" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="Y55" s="2" t="s">
+      <c r="Z55" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="Z55" s="2" t="s">
+      <c r="AA55" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3796,23 +4110,26 @@
       <c r="C56" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E56" s="1">
+      <c r="D56" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F56" s="1">
         <v>17</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="Q56" s="1">
+      <c r="R56" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>58</v>
       </c>
@@ -3822,49 +4139,52 @@
       <c r="C57" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D57" s="1">
-        <v>1</v>
+      <c r="D57" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
         <v>17</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="Q57" s="1">
-        <v>1</v>
-      </c>
       <c r="R57" s="1">
+        <v>1</v>
+      </c>
+      <c r="S57" s="1">
         <v>9</v>
       </c>
-      <c r="S57" s="1" t="s">
+      <c r="T57" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="T57" s="1" t="s">
+      <c r="U57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U57" s="2" t="s">
+      <c r="V57" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="W57" s="2" t="s">
+      <c r="X57" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="Y57" s="2" t="s">
+      <c r="Z57" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="Z57" s="2" t="s">
+      <c r="AA57" s="2" t="s">
         <v>197</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Z57">
-    <sortCondition ref="E2:E57"/>
+  <sortState ref="A2:AA57">
+    <sortCondition ref="F2:F57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add hub item id to profile builder
</commit_message>
<xml_diff>
--- a/unsd/country-profiles/ProjectCountryProfilesPython/CountryProfileBuilder.xlsx
+++ b/unsd/country-profiles/ProjectCountryProfilesPython/CountryProfileBuilder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\unsd\country-profiles\ProjectCountryProfilesPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68BFC46-C238-40A8-AA30-7ECCCFD4B098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704E2720-9B5E-4513-8EB5-4BFAC493C310}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" xr2:uid="{608E191F-5FEB-4D0E-811F-33218E7FD720}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CountryProfileBuilder" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AG$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AH$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="346">
   <si>
     <t>No.</t>
   </si>
@@ -930,6 +930,147 @@
   </si>
   <si>
     <t>Up</t>
+  </si>
+  <si>
+    <t>ed6ee35ad584405b8f3ef2abc22f6948</t>
+  </si>
+  <si>
+    <t>HubItemId</t>
+  </si>
+  <si>
+    <t>deb1f4a7e2e14d78a113c53cba2838de</t>
+  </si>
+  <si>
+    <t>f4cb37d065aa4b6981d93e8266f63fd0</t>
+  </si>
+  <si>
+    <t>8c0866ad73ae486ba647f5490fed5529</t>
+  </si>
+  <si>
+    <t>30ea76b4f4094d4aa7645a213ccaa4b9</t>
+  </si>
+  <si>
+    <t>65925035bb984f66aa03480f6754c4fe</t>
+  </si>
+  <si>
+    <t>a012070afbd3486d9c0596352b9698d6</t>
+  </si>
+  <si>
+    <t>216c7516b9444f289e8f7910c8726e9f</t>
+  </si>
+  <si>
+    <t>954b5087e440421ba26a3213c99d9a9f</t>
+  </si>
+  <si>
+    <t>1a967f6f5fe64fc5b27f49a5c20e4fe4</t>
+  </si>
+  <si>
+    <t>0c846dfa5bab411c9a1a21ae40dd0232</t>
+  </si>
+  <si>
+    <t>dc8f11cd784344f18d0478072691b943</t>
+  </si>
+  <si>
+    <t>512b7b1d05a14b90853ea5ca1d003b1b</t>
+  </si>
+  <si>
+    <t>c24e8fbbada54780b6c36fd899f864b2</t>
+  </si>
+  <si>
+    <t>7f75a26e77c7487e993799b22ad7ba88</t>
+  </si>
+  <si>
+    <t>8f2dd8895e1242db8ef4ca25415d609d</t>
+  </si>
+  <si>
+    <t>3459681b792a4979a9d9731c75f7f80d</t>
+  </si>
+  <si>
+    <t>32abbaca0c3a47c0aae18f50bd7e8f56</t>
+  </si>
+  <si>
+    <t>337524c727bd498c8726f9f6bc6512e1</t>
+  </si>
+  <si>
+    <t>2186448878244705a5295710c140b8c3</t>
+  </si>
+  <si>
+    <t>8f37f35525db476a9da37c7d83beffa9</t>
+  </si>
+  <si>
+    <t>28a9a3072fd940aa9fb0f983d25ef65f</t>
+  </si>
+  <si>
+    <t>9fd0677f368c48dca6f5e11f64badafd</t>
+  </si>
+  <si>
+    <t>b087399f0b874ab9948714edcd49cbdd</t>
+  </si>
+  <si>
+    <t>81cf3e70351c4895828a2486efa2142c</t>
+  </si>
+  <si>
+    <t>3cb997d2497148e68dca6787fcb84ca5</t>
+  </si>
+  <si>
+    <t>72c32323563d4a0b9432c9edcb85267a</t>
+  </si>
+  <si>
+    <t>b5ff535a5fa841659c576685489dfac7</t>
+  </si>
+  <si>
+    <t>a4e6d6a6cc804c3598cc9b96cd96ce67</t>
+  </si>
+  <si>
+    <t>8943ce6f81b44120b6124fedb3b094d8</t>
+  </si>
+  <si>
+    <t>635cd0cae73e4b2dae2661407be6eeec</t>
+  </si>
+  <si>
+    <t>5b43bb59961a46daa3b8af9384f60103</t>
+  </si>
+  <si>
+    <t>f158f819bd284fd5b35e456a152a069c</t>
+  </si>
+  <si>
+    <t>995242b2ec9f4a21975ef7d47b5657bb</t>
+  </si>
+  <si>
+    <t>9c33807e2ddf4e348737fab085de0ac1</t>
+  </si>
+  <si>
+    <t>d675ccc2f7054d82b371e64fb2cbface</t>
+  </si>
+  <si>
+    <t>2a0cad7f76284e8c978bfcb0fa15cd76</t>
+  </si>
+  <si>
+    <t>e23061ce674142b5b33c46ea5e031658</t>
+  </si>
+  <si>
+    <t>5c12290ecd1c4a49bc3734721d941d10</t>
+  </si>
+  <si>
+    <t>c2c0216c53744dd7b5278e398328bc99</t>
+  </si>
+  <si>
+    <t>b65e89e905a744e5992889ddc27f8fc7</t>
+  </si>
+  <si>
+    <t>f16a0c0c54504a84bd7296f42375d73e</t>
+  </si>
+  <si>
+    <t>f59cf3f8a0ec41a2b601a28682e6f2c8</t>
+  </si>
+  <si>
+    <t>bc201a5c69e94e23b45bad86c828f1be</t>
+  </si>
+  <si>
+    <t>4da2587ef9094c7bb1e2980644211cf2</t>
+  </si>
+  <si>
+    <t>68e9ec78abe543889762bbdd36cd3d31</t>
   </si>
 </sst>
 </file>
@@ -945,12 +1086,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -965,13 +1112,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,38 +1437,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BF65AC-2E6C-4B3F-8D19-434C6AC10D50}">
-  <dimension ref="A1:Z57"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection sqref="A1:AA57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="56.85546875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="56.85546875" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1329,76 +1480,79 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1408,47 +1562,50 @@
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
+      <c r="D2" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="1">
-        <v>1</v>
-      </c>
       <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>26</v>
+      <c r="S2" s="1">
+        <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1458,53 +1615,56 @@
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
+      <c r="D3" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
       <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
         <v>2</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1514,47 +1674,50 @@
       <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
+      <c r="D4" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
       <c r="R4" s="1">
         <v>1</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1564,53 +1727,56 @@
       <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
+      <c r="D5" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="1">
-        <v>1</v>
-      </c>
       <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
         <v>2</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1620,26 +1786,29 @@
       <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1649,47 +1818,50 @@
       <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
+      <c r="D7" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <v>0</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>7</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="U7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="AA7" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1699,53 +1871,56 @@
       <c r="C8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
+      <c r="D8" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="1">
-        <v>1</v>
-      </c>
       <c r="R8" s="1">
         <v>1</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>26</v>
+      <c r="S8" s="1">
+        <v>1</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="U8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1755,53 +1930,56 @@
       <c r="C9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
+      <c r="D9" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <v>0</v>
       </c>
-      <c r="R9" s="1">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1" t="s">
+      <c r="S9" s="1">
+        <v>1</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="AA9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1811,53 +1989,56 @@
       <c r="C10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
+      <c r="D10" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="1">
-        <v>1</v>
-      </c>
       <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
         <v>13</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="Y10" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1867,23 +2048,26 @@
       <c r="C11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="1">
+      <c r="D11" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1893,47 +2077,50 @@
       <c r="C12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
+      <c r="D12" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <v>0</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>14</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="X12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Z12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z12" s="2" t="s">
+      <c r="AA12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1943,23 +2130,26 @@
       <c r="C13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="1">
+      <c r="D13" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>56</v>
       </c>
@@ -1969,50 +2159,53 @@
       <c r="C14" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
+      <c r="D14" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <v>0</v>
       </c>
-      <c r="R14" s="1">
-        <v>1</v>
-      </c>
-      <c r="S14" s="1" t="s">
+      <c r="S14" s="1">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="AA14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2022,44 +2215,47 @@
       <c r="C15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="1">
-        <v>1</v>
+      <c r="D15" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
         <v>4</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>0</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>4</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="V15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="V15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="Y15" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2069,44 +2265,47 @@
       <c r="C16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="1">
-        <v>1</v>
+      <c r="D16" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>0</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <v>4</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="V16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="V16" s="2" t="s">
+      <c r="W16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="X16" s="2" t="s">
+      <c r="Y16" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2116,44 +2315,47 @@
       <c r="C17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="1">
+      <c r="D17" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F17" s="1">
         <v>4</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <v>0</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="V17" s="2" t="s">
+      <c r="W17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Y17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="AA17" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>57</v>
       </c>
@@ -2163,47 +2365,50 @@
       <c r="C18" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D18" s="1">
-        <v>1</v>
+      <c r="D18" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
         <v>4</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <v>0</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <v>2</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="V18" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="AA18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -2213,26 +2418,29 @@
       <c r="C19" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="1">
+      <c r="D19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F19" s="1">
         <v>5</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="R19" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -2242,47 +2450,50 @@
       <c r="C20" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="1">
-        <v>1</v>
+      <c r="D20" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
         <v>5</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <v>0</v>
       </c>
-      <c r="R20" s="1">
-        <v>1</v>
-      </c>
-      <c r="S20" s="1" t="s">
+      <c r="S20" s="1">
+        <v>1</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="V20" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="X20" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="Y20" s="2" t="s">
+      <c r="Z20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z20" s="2" t="s">
+      <c r="AA20" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2292,50 +2503,53 @@
       <c r="C21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="1">
-        <v>1</v>
+      <c r="D21" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
         <v>5</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <v>0</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S21" s="1">
         <v>2</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="V21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="X21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z21" s="2" t="s">
+      <c r="AA21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2345,26 +2559,29 @@
       <c r="C22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="1">
+      <c r="D22" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F22" s="1">
         <v>6</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -2374,44 +2591,47 @@
       <c r="C23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="1">
+      <c r="D23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F23" s="1">
         <v>6</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q23" s="1">
-        <v>1</v>
-      </c>
       <c r="R23" s="1">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1">
         <v>2</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="V23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Z23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z23" s="2" t="s">
+      <c r="AA23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2421,26 +2641,29 @@
       <c r="C24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="1">
+      <c r="D24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F24" s="1">
         <v>6</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -2450,32 +2673,35 @@
       <c r="C25" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="1">
+      <c r="D25" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" s="1">
         <v>6</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="R25" s="1">
         <v>0</v>
       </c>
-      <c r="Y25" s="2" t="s">
+      <c r="Z25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z25" s="2" t="s">
+      <c r="AA25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -2485,47 +2711,50 @@
       <c r="C26" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="1">
-        <v>1</v>
+      <c r="D26" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
         <v>6</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="R26" s="1">
         <v>0</v>
       </c>
-      <c r="R26" s="1">
+      <c r="S26" s="1">
         <v>2</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="V26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="W26" s="2" t="s">
+      <c r="X26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Y26" s="2" t="s">
+      <c r="Z26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z26" s="2" t="s">
+      <c r="AA26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -2535,26 +2764,29 @@
       <c r="C27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="1">
+      <c r="D27" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F27" s="1">
         <v>6</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -2564,47 +2796,50 @@
       <c r="C28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="1">
-        <v>1</v>
+      <c r="D28" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
         <v>6</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="R28" s="1">
         <v>0</v>
       </c>
-      <c r="R28" s="1">
+      <c r="S28" s="1">
         <v>2</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="V28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W28" s="2" t="s">
+      <c r="X28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="Y28" s="2" t="s">
+      <c r="Z28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z28" s="2" t="s">
+      <c r="AA28" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -2614,38 +2849,41 @@
       <c r="C29" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D29" s="1">
-        <v>1</v>
+      <c r="D29" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="R29" s="1">
         <v>0</v>
       </c>
-      <c r="R29" s="1">
+      <c r="S29" s="1">
         <v>8</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="V29" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="W29" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -2655,47 +2893,50 @@
       <c r="C30" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="1">
-        <v>1</v>
+      <c r="D30" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
         <v>7</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="R30" s="1">
         <v>0</v>
       </c>
-      <c r="R30" s="1">
-        <v>1</v>
-      </c>
-      <c r="S30" s="1" t="s">
+      <c r="S30" s="1">
+        <v>1</v>
+      </c>
+      <c r="T30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="V30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="W30" s="2" t="s">
+      <c r="X30" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="Y30" s="2" t="s">
+      <c r="Z30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z30" s="2" t="s">
+      <c r="AA30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2705,44 +2946,47 @@
       <c r="C31" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="1">
-        <v>1</v>
+      <c r="D31" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
         <v>8</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="R31" s="1">
         <v>0</v>
       </c>
-      <c r="R31" s="1">
-        <v>1</v>
-      </c>
-      <c r="S31" s="1" t="s">
+      <c r="S31" s="1">
+        <v>1</v>
+      </c>
+      <c r="T31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="V31" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="W31" s="2" t="s">
+      <c r="X31" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y31" s="2" t="s">
+      <c r="Z31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z31" s="2" t="s">
+      <c r="AA31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2752,29 +2996,32 @@
       <c r="C32" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E32" s="1">
+      <c r="D32" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F32" s="1">
         <v>8</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="R32" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2784,29 +3031,32 @@
       <c r="C33" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E33" s="1">
+      <c r="D33" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F33" s="1">
         <v>8</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="R33" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2816,29 +3066,32 @@
       <c r="C34" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E34" s="1">
+      <c r="D34" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F34" s="1">
         <v>8</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="R34" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2848,50 +3101,53 @@
       <c r="C35" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D35" s="1">
-        <v>1</v>
+      <c r="D35" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
         <v>8</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="R35" s="1">
         <v>0</v>
       </c>
-      <c r="R35" s="1">
-        <v>1</v>
-      </c>
-      <c r="S35" s="1" t="s">
+      <c r="S35" s="1">
+        <v>1</v>
+      </c>
+      <c r="T35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U35" s="2" t="s">
+      <c r="V35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="W35" s="2" t="s">
+      <c r="X35" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="Y35" s="2" t="s">
+      <c r="Z35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z35" s="2" t="s">
+      <c r="AA35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2901,29 +3157,32 @@
       <c r="C36" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E36" s="1">
+      <c r="D36" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F36" s="1">
         <v>8</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="R36" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2933,44 +3192,47 @@
       <c r="C37" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D37" s="1">
-        <v>1</v>
+      <c r="D37" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
         <v>9</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="R37" s="1">
         <v>0</v>
       </c>
-      <c r="R37" s="1">
-        <v>1</v>
-      </c>
-      <c r="S37" s="1" t="s">
+      <c r="S37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="V37" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="W37" s="2" t="s">
+      <c r="X37" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Y37" s="2" t="s">
+      <c r="Z37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z37" s="2" t="s">
+      <c r="AA37" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2980,47 +3242,50 @@
       <c r="C38" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D38" s="1">
-        <v>1</v>
+      <c r="D38" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
         <v>9</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="R38" s="1">
         <v>0</v>
       </c>
-      <c r="R38" s="1">
+      <c r="S38" s="1">
         <v>9</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="U38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U38" s="2" t="s">
+      <c r="V38" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="W38" s="2" t="s">
+      <c r="X38" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="Y38" s="2" t="s">
+      <c r="Z38" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Z38" s="2" t="s">
+      <c r="AA38" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3030,47 +3295,50 @@
       <c r="C39" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D39" s="1">
-        <v>1</v>
+      <c r="D39" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
         <v>9</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="R39" s="1">
         <v>0</v>
       </c>
-      <c r="R39" s="1">
+      <c r="S39" s="1">
         <v>2</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U39" s="2" t="s">
+      <c r="V39" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="W39" s="2" t="s">
+      <c r="X39" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="Y39" s="2" t="s">
+      <c r="Z39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z39" s="2" t="s">
+      <c r="AA39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -3080,44 +3348,47 @@
       <c r="C40" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D40" s="1">
-        <v>1</v>
+      <c r="D40" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
         <v>10</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="R40" s="1">
         <v>0</v>
       </c>
-      <c r="R40" s="1">
+      <c r="S40" s="1">
         <v>2</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U40" s="2" t="s">
+      <c r="V40" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W40" s="2" t="s">
+      <c r="X40" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="Y40" s="2" t="s">
+      <c r="Z40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Z40" s="2" t="s">
+      <c r="AA40" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -3127,47 +3398,50 @@
       <c r="C41" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D41" s="1">
-        <v>1</v>
+      <c r="D41" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
         <v>11</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="R41" s="1">
         <v>0</v>
       </c>
-      <c r="R41" s="1">
+      <c r="S41" s="1">
         <v>10</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="U41" s="2" t="s">
+      <c r="V41" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="W41" s="2" t="s">
+      <c r="X41" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="Y41" s="2" t="s">
+      <c r="Z41" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="Z41" s="2" t="s">
+      <c r="AA41" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -3177,26 +3451,29 @@
       <c r="C42" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E42" s="1">
+      <c r="D42" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F42" s="1">
         <v>11</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="R42" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -3206,44 +3483,47 @@
       <c r="C43" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D43" s="1">
-        <v>1</v>
+      <c r="D43" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
         <v>11</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="R43" s="1">
         <v>0</v>
       </c>
-      <c r="R43" s="1">
-        <v>1</v>
-      </c>
-      <c r="S43" s="1" t="s">
+      <c r="S43" s="1">
+        <v>1</v>
+      </c>
+      <c r="T43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U43" s="2" t="s">
+      <c r="V43" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W43" s="2" t="s">
+      <c r="X43" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="Y43" s="2" t="s">
+      <c r="Z43" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="Z43" s="2" t="s">
+      <c r="AA43" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>28</v>
       </c>
@@ -3253,47 +3533,50 @@
       <c r="C44" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D44" s="1">
-        <v>1</v>
+      <c r="D44" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
         <v>12</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="Q44" s="1">
-        <v>1</v>
-      </c>
       <c r="R44" s="1">
         <v>1</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="S44" s="1">
+        <v>1</v>
+      </c>
+      <c r="T44" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="U44" s="2" t="s">
+      <c r="V44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="W44" s="2" t="s">
+      <c r="X44" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="Y44" s="2" t="s">
+      <c r="Z44" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Z44" s="2" t="s">
+      <c r="AA44" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>29</v>
       </c>
@@ -3303,38 +3586,41 @@
       <c r="C45" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E45" s="1">
+      <c r="D45" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F45" s="1">
         <v>12</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="Q45" s="1">
-        <v>1</v>
-      </c>
       <c r="R45" s="1">
+        <v>1</v>
+      </c>
+      <c r="S45" s="1">
         <v>7</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="V45" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="W45" s="2" t="s">
+      <c r="X45" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>55</v>
       </c>
@@ -3344,38 +3630,41 @@
       <c r="C46" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D46" s="1">
-        <v>1</v>
+      <c r="D46" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
         <v>13</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="R46" s="1">
         <v>0</v>
       </c>
-      <c r="R46" s="1">
+      <c r="S46" s="1">
         <v>12</v>
       </c>
-      <c r="W46" s="2" t="s">
+      <c r="X46" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="Y46" s="2" t="s">
+      <c r="Z46" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="Z46" s="2" t="s">
+      <c r="AA46" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44</v>
       </c>
@@ -3385,38 +3674,41 @@
       <c r="C47" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D47" s="1">
-        <v>1</v>
+      <c r="D47" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
         <v>14</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="Q47" s="1">
-        <v>1</v>
-      </c>
       <c r="R47" s="1">
+        <v>1</v>
+      </c>
+      <c r="S47" s="1">
         <v>8</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="V47" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="X47" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45</v>
       </c>
@@ -3426,44 +3718,47 @@
       <c r="C48" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D48" s="1">
-        <v>1</v>
+      <c r="D48" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
         <v>15</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="Q48" s="1">
-        <v>1</v>
-      </c>
       <c r="R48" s="1">
         <v>1</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="S48" s="1">
+        <v>1</v>
+      </c>
+      <c r="T48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="V48" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="W48" s="2" t="s">
+      <c r="X48" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="Y48" s="2" t="s">
+      <c r="Z48" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="Z48" s="2" t="s">
+      <c r="AA48" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -3473,41 +3768,44 @@
       <c r="C49" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D49" s="1">
-        <v>1</v>
+      <c r="D49" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
         <v>15</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q49" s="1">
-        <v>1</v>
-      </c>
       <c r="R49" s="1">
+        <v>1</v>
+      </c>
+      <c r="S49" s="1">
         <v>7</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U49" s="2" t="s">
+      <c r="V49" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="W49" s="2" t="s">
+      <c r="X49" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3517,41 +3815,44 @@
       <c r="C50" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D50" s="1">
-        <v>1</v>
+      <c r="D50" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
         <v>15</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q50" s="1">
-        <v>1</v>
-      </c>
       <c r="R50" s="1">
+        <v>1</v>
+      </c>
+      <c r="S50" s="1">
         <v>7</v>
       </c>
-      <c r="S50" s="1" t="s">
+      <c r="T50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U50" s="2" t="s">
+      <c r="V50" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="W50" s="2" t="s">
+      <c r="X50" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3561,47 +3862,48 @@
       <c r="C51" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
+      <c r="D51" s="3"/>
       <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
         <v>16</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q51" s="1">
+      <c r="R51" s="1">
         <v>0</v>
       </c>
-      <c r="R51" s="1">
+      <c r="S51" s="1">
         <v>3</v>
       </c>
-      <c r="S51" s="1" t="s">
+      <c r="T51" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U51" s="2" t="s">
+      <c r="V51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="V51" s="2" t="s">
+      <c r="W51" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="W51" s="2" t="s">
+      <c r="X51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="X51" s="2" t="s">
+      <c r="Y51" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3611,38 +3913,41 @@
       <c r="C52" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D52" s="1">
-        <v>1</v>
+      <c r="D52" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
         <v>16</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="R52" s="1">
         <v>0</v>
       </c>
-      <c r="R52" s="1">
+      <c r="S52" s="1">
         <v>11</v>
       </c>
-      <c r="S52" s="1" t="s">
+      <c r="T52" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="U52" s="2" t="s">
+      <c r="V52" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="W52" s="2" t="s">
+      <c r="X52" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3652,47 +3957,50 @@
       <c r="C53" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D53" s="1">
-        <v>1</v>
+      <c r="D53" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
         <v>17</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="Q53" s="1">
-        <v>1</v>
-      </c>
       <c r="R53" s="1">
         <v>1</v>
       </c>
-      <c r="S53" s="1" t="s">
-        <v>26</v>
+      <c r="S53" s="1">
+        <v>1</v>
       </c>
       <c r="T53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U53" s="2" t="s">
+      <c r="U53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V53" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="W53" s="2" t="s">
+      <c r="X53" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="Y53" s="2" t="s">
+      <c r="Z53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z53" s="2" t="s">
+      <c r="AA53" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3702,50 +4010,53 @@
       <c r="C54" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D54" s="1">
-        <v>1</v>
+      <c r="D54" s="1" t="s">
+        <v>342</v>
       </c>
       <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
         <v>17</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="P54" s="1" t="s">
+      <c r="Q54" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="Q54" s="1">
+      <c r="R54" s="1">
         <v>0</v>
       </c>
-      <c r="R54" s="1">
+      <c r="S54" s="1">
         <v>15</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="T54" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U54" s="2" t="s">
+      <c r="V54" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="W54" s="2" t="s">
+      <c r="X54" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="Y54" s="2" t="s">
+      <c r="Z54" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Z54" s="2" t="s">
+      <c r="AA54" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3755,38 +4066,41 @@
       <c r="C55" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D55" s="1">
-        <v>1</v>
+      <c r="D55" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
         <v>17</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="Q55" s="1">
+      <c r="R55" s="1">
         <v>0</v>
       </c>
-      <c r="R55" s="1">
+      <c r="S55" s="1">
         <v>12</v>
       </c>
-      <c r="W55" s="2" t="s">
+      <c r="X55" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="Y55" s="2" t="s">
+      <c r="Z55" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="Z55" s="2" t="s">
+      <c r="AA55" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3796,23 +4110,26 @@
       <c r="C56" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E56" s="1">
+      <c r="D56" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F56" s="1">
         <v>17</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="Q56" s="1">
+      <c r="R56" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>58</v>
       </c>
@@ -3822,49 +4139,52 @@
       <c r="C57" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D57" s="1">
-        <v>1</v>
+      <c r="D57" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
         <v>17</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="Q57" s="1">
-        <v>1</v>
-      </c>
       <c r="R57" s="1">
+        <v>1</v>
+      </c>
+      <c r="S57" s="1">
         <v>9</v>
       </c>
-      <c r="S57" s="1" t="s">
+      <c r="T57" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="T57" s="1" t="s">
+      <c r="U57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U57" s="2" t="s">
+      <c r="V57" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="W57" s="2" t="s">
+      <c r="X57" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="Y57" s="2" t="s">
+      <c r="Z57" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="Z57" s="2" t="s">
+      <c r="AA57" s="2" t="s">
         <v>197</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Z57">
-    <sortCondition ref="E2:E57"/>
+  <sortState ref="A2:AA57">
+    <sortCondition ref="F2:F57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
svg files for icons
</commit_message>
<xml_diff>
--- a/unsd/country-profiles/ProjectCountryProfilesPython/CountryProfileBuilder.xlsx
+++ b/unsd/country-profiles/ProjectCountryProfilesPython/CountryProfileBuilder.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\unsd\country-profiles\ProjectCountryProfilesPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704E2720-9B5E-4513-8EB5-4BFAC493C310}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2399F45-0418-43CC-87D9-306AB639D25D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" xr2:uid="{608E191F-5FEB-4D0E-811F-33218E7FD720}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryProfileBuilder" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AH$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">Sheet1!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="346">
   <si>
     <t>No.</t>
   </si>
@@ -1439,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BF65AC-2E6C-4B3F-8D19-434C6AC10D50}">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection sqref="A1:AA57"/>
+    <sheetView tabSelected="1" topLeftCell="H14" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4188,4 +4191,262 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7797A2-432F-403E-917F-B7361970241F}">
+  <dimension ref="A1:A48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>